<commit_message>
Complete Results with Chart
</commit_message>
<xml_diff>
--- a/Nitheesha/completeResults.xlsx
+++ b/Nitheesha/completeResults.xlsx
@@ -15,22 +15,19 @@
     <sheet name="completeResults" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">completeResults!$A$1:$B$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">completeResults!$A$1:$B$27</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Year</t>
   </si>
   <si>
     <t>salesTotal</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -700,10 +697,11 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>completeResults!$A$2:$A$28</c:f>
-              <c:strCache>
-                <c:ptCount val="27"/>
+            <c:numRef>
+              <c:f>completeResults!$A$2:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1985</c:v>
                 </c:pt>
@@ -782,18 +780,15 @@
                 <c:pt idx="25">
                   <c:v>2020</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>N/A</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>completeResults!$B$2:$B$28</c:f>
+              <c:f>completeResults!$B$2:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
@@ -871,9 +866,6 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0.57999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>148.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -889,11 +881,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="281672592"/>
-        <c:axId val="281675728"/>
+        <c:axId val="347586768"/>
+        <c:axId val="280810376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="281672592"/>
+        <c:axId val="347586768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,7 +928,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281675728"/>
+        <c:crossAx val="280810376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -944,7 +936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="281675728"/>
+        <c:axId val="280810376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -995,7 +987,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281672592"/>
+        <c:crossAx val="347586768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1885,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,16 +2105,8 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="2">
-        <v>148.22</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B28"/>
+  <autoFilter ref="A1:B27"/>
   <sortState ref="A2:B28">
     <sortCondition ref="A1"/>
   </sortState>

</xml_diff>